<commit_message>
Updated the stream walks to include a plot with the two years and all of the counts summed accross streams.
</commit_message>
<xml_diff>
--- a/VisualSurvey_RImport.xlsx
+++ b/VisualSurvey_RImport.xlsx
@@ -778,11 +778,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q241"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K146" sqref="K146"/>
+      <selection pane="bottomLeft" activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,7 +858,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>41423</v>
       </c>
@@ -877,7 +878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>41423</v>
       </c>
@@ -900,7 +901,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>41423</v>
       </c>
@@ -943,7 +944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>41430</v>
       </c>
@@ -963,7 +964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>41430</v>
       </c>
@@ -983,7 +984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>41430</v>
       </c>
@@ -1023,7 +1024,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>41436</v>
       </c>
@@ -1046,7 +1047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>41436</v>
       </c>
@@ -1066,7 +1067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>41436</v>
       </c>
@@ -1106,7 +1107,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>41443</v>
       </c>
@@ -1126,7 +1127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>41443</v>
       </c>
@@ -1152,7 +1153,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>41443</v>
       </c>
@@ -1201,7 +1202,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>41457</v>
       </c>
@@ -1221,7 +1222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>41457</v>
       </c>
@@ -1241,7 +1242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>41457</v>
       </c>
@@ -1281,7 +1282,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>41464</v>
       </c>
@@ -1301,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>41464</v>
       </c>
@@ -1321,7 +1322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>41464</v>
       </c>
@@ -1361,7 +1362,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>41471</v>
       </c>
@@ -1384,7 +1385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>41471</v>
       </c>
@@ -1407,7 +1408,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>41471</v>
       </c>
@@ -1450,7 +1451,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>41509</v>
       </c>
@@ -1476,7 +1477,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>41509</v>
       </c>
@@ -1496,7 +1497,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>41515</v>
       </c>
@@ -1519,7 +1520,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>41515</v>
       </c>
@@ -1562,7 +1563,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>41523</v>
       </c>
@@ -1582,7 +1583,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>41523</v>
       </c>
@@ -1622,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>41773</v>
       </c>
@@ -1650,7 +1651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>41773</v>
       </c>
@@ -1678,7 +1679,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>41773</v>
       </c>
@@ -1706,7 +1707,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>41773</v>
       </c>
@@ -1734,7 +1735,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>41773</v>
       </c>
@@ -1762,7 +1763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>41773</v>
       </c>
@@ -1818,7 +1819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>41773</v>
       </c>
@@ -1846,7 +1847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>41779</v>
       </c>
@@ -1876,7 +1877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>41779</v>
       </c>
@@ -1906,7 +1907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>41779</v>
       </c>
@@ -1936,7 +1937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>41779</v>
       </c>
@@ -1966,7 +1967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>41779</v>
       </c>
@@ -1996,7 +1997,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>41779</v>
       </c>
@@ -2056,7 +2057,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>41786</v>
       </c>
@@ -2084,7 +2085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>41786</v>
       </c>
@@ -2115,7 +2116,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>41786</v>
       </c>
@@ -2143,7 +2144,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>41786</v>
       </c>
@@ -2171,7 +2172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>41786</v>
       </c>
@@ -2199,7 +2200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>41786</v>
       </c>
@@ -2255,7 +2256,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>41802</v>
       </c>
@@ -2282,7 +2283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>41802</v>
       </c>
@@ -2309,7 +2310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>41802</v>
       </c>
@@ -2336,7 +2337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>41802</v>
       </c>
@@ -2390,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>41802</v>
       </c>
@@ -2418,7 +2419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>41810</v>
       </c>
@@ -2448,7 +2449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>41810</v>
       </c>
@@ -2478,7 +2479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>41810</v>
       </c>
@@ -2508,7 +2509,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>41810</v>
       </c>
@@ -2571,7 +2572,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>41810</v>
       </c>
@@ -2604,7 +2605,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>41870</v>
       </c>
@@ -2639,7 +2640,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>41870</v>
       </c>
@@ -2677,7 +2678,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>41870</v>
       </c>
@@ -2712,7 +2713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>41870</v>
       </c>
@@ -2747,7 +2748,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>41870</v>
       </c>
@@ -2785,7 +2786,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>41870</v>
       </c>
@@ -2858,7 +2859,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>41870</v>
       </c>
@@ -2896,7 +2897,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>41877</v>
       </c>
@@ -2928,7 +2929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>41877</v>
       </c>
@@ -2960,7 +2961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>41877</v>
       </c>
@@ -2992,7 +2993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>41877</v>
       </c>
@@ -3024,7 +3025,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="84" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>41877</v>
       </c>
@@ -3059,7 +3060,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="85" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>41877</v>
       </c>
@@ -3123,7 +3124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>41877</v>
       </c>
@@ -3155,7 +3156,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>41885</v>
       </c>
@@ -3190,7 +3191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>41885</v>
       </c>
@@ -3225,7 +3226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>41885</v>
       </c>
@@ -3260,7 +3261,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="91" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>41885</v>
       </c>
@@ -3295,7 +3296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>41885</v>
       </c>
@@ -3368,7 +3369,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>41885</v>
       </c>
@@ -3406,7 +3407,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>41892</v>
       </c>
@@ -3444,7 +3445,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>41892</v>
       </c>
@@ -3482,7 +3483,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>41892</v>
       </c>
@@ -3517,7 +3518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>41892</v>
       </c>
@@ -3552,7 +3553,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>41892</v>
       </c>
@@ -3587,7 +3588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>41892</v>
       </c>
@@ -3660,7 +3661,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>41892</v>
       </c>
@@ -3695,7 +3696,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>41898</v>
       </c>
@@ -3730,7 +3731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>41898</v>
       </c>
@@ -3765,7 +3766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>41898</v>
       </c>
@@ -3800,7 +3801,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>41898</v>
       </c>
@@ -3838,7 +3839,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>41898</v>
       </c>
@@ -3908,7 +3909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>41898</v>
       </c>
@@ -3946,7 +3947,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>41905</v>
       </c>
@@ -3978,7 +3979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>41905</v>
       </c>
@@ -4010,7 +4011,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>41905</v>
       </c>
@@ -4042,7 +4043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>41905</v>
       </c>
@@ -4106,7 +4107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>41905</v>
       </c>
@@ -4138,7 +4139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>41913</v>
       </c>
@@ -4170,7 +4171,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>41913</v>
       </c>
@@ -4202,7 +4203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>41913</v>
       </c>
@@ -4234,7 +4235,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>41913</v>
       </c>
@@ -4266,7 +4267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>41913</v>
       </c>
@@ -4330,7 +4331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>41913</v>
       </c>
@@ -4362,7 +4363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>42132</v>
       </c>
@@ -4380,7 +4381,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="124" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>42132</v>
       </c>
@@ -4423,7 +4424,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="125" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>42132</v>
       </c>
@@ -4463,7 +4464,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>42132</v>
       </c>
@@ -4503,7 +4504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>42132</v>
       </c>
@@ -4543,7 +4544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>42132</v>
       </c>
@@ -4623,7 +4624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>42139</v>
       </c>
@@ -4663,7 +4664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>42139</v>
       </c>
@@ -4703,7 +4704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>42139</v>
       </c>
@@ -4743,7 +4744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>42139</v>
       </c>
@@ -4783,7 +4784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>42139</v>
       </c>
@@ -4863,7 +4864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>42152</v>
       </c>
@@ -4903,7 +4904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>42152</v>
       </c>
@@ -4943,7 +4944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>42152</v>
       </c>
@@ -4983,7 +4984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>42152</v>
       </c>
@@ -5023,7 +5024,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>42152</v>
       </c>
@@ -5106,7 +5107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>42160</v>
       </c>
@@ -5153,7 +5154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
         <v>42160</v>
       </c>
@@ -5200,7 +5201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
         <v>42160</v>
       </c>
@@ -5294,7 +5295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
         <v>42160</v>
       </c>
@@ -5341,7 +5342,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="147" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
         <v>42160</v>
       </c>
@@ -5388,7 +5389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
         <v>42167</v>
       </c>
@@ -5438,7 +5439,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="149" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
         <v>42167</v>
       </c>
@@ -5485,7 +5486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
         <v>42167</v>
       </c>
@@ -5579,7 +5580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
         <v>42167</v>
       </c>
@@ -5626,7 +5627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
         <v>42167</v>
       </c>
@@ -5673,7 +5674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
         <v>42174</v>
       </c>
@@ -5717,7 +5718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
         <v>42174</v>
       </c>
@@ -5761,7 +5762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
         <v>42174</v>
       </c>
@@ -5849,7 +5850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
         <v>42174</v>
       </c>
@@ -5893,7 +5894,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
         <v>42174</v>
       </c>
@@ -5938,7 +5939,7 @@
       </c>
       <c r="Q159" s="7"/>
     </row>
-    <row r="160" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
         <v>42181</v>
       </c>
@@ -5986,7 +5987,7 @@
       </c>
       <c r="Q160" s="7"/>
     </row>
-    <row r="161" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
         <v>42181</v>
       </c>
@@ -6033,7 +6034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
         <v>42181</v>
       </c>
@@ -6127,7 +6128,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
         <v>42181</v>
       </c>
@@ -6174,7 +6175,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
         <v>42181</v>
       </c>
@@ -6221,7 +6222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
         <v>42181</v>
       </c>
@@ -6268,7 +6269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="8">
         <v>42229</v>
       </c>
@@ -6317,7 +6318,7 @@
       </c>
       <c r="Q167" s="6"/>
     </row>
-    <row r="168" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="8">
         <v>42229</v>
       </c>
@@ -6366,7 +6367,7 @@
       </c>
       <c r="Q168" s="6"/>
     </row>
-    <row r="169" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="8">
         <v>42229</v>
       </c>
@@ -6458,7 +6459,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="171" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="8">
         <v>42229</v>
       </c>
@@ -6501,7 +6502,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="172" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="8">
         <v>42229</v>
       </c>
@@ -6544,7 +6545,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="173" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173" s="8">
         <v>42229</v>
       </c>
@@ -6587,7 +6588,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="174" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="8">
         <v>42229</v>
       </c>
@@ -6630,7 +6631,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="175" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="8">
         <v>42237</v>
       </c>
@@ -6674,7 +6675,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="176" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="8">
         <v>42237</v>
       </c>
@@ -6723,7 +6724,7 @@
       </c>
       <c r="Q176" s="6"/>
     </row>
-    <row r="177" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="8">
         <v>42237</v>
       </c>
@@ -6817,7 +6818,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="179" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179" s="8">
         <v>42237</v>
       </c>
@@ -6860,7 +6861,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="180" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180" s="8">
         <v>42237</v>
       </c>
@@ -6903,7 +6904,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="181" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181" s="8">
         <v>42237</v>
       </c>
@@ -6946,7 +6947,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="182" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182" s="8">
         <v>42237</v>
       </c>
@@ -6989,7 +6990,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="183" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="8">
         <v>42244</v>
       </c>
@@ -7033,7 +7034,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="184" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="8">
         <v>42244</v>
       </c>
@@ -7071,7 +7072,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="185" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185" s="8">
         <v>42244</v>
       </c>
@@ -7161,7 +7162,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="187" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="8">
         <v>42244</v>
       </c>
@@ -7200,7 +7201,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="188" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="8">
         <v>42244</v>
       </c>
@@ -7239,7 +7240,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="189" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189" s="8">
         <v>42244</v>
       </c>
@@ -7277,7 +7278,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="190" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190" s="8">
         <v>42244</v>
       </c>
@@ -7315,7 +7316,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="191" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191" s="3">
         <v>42251</v>
       </c>
@@ -7332,7 +7333,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="192" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192" s="3">
         <v>42251</v>
       </c>
@@ -7384,7 +7385,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="193" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193" s="3">
         <v>42251</v>
       </c>
@@ -7475,7 +7476,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="195" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195" s="3">
         <v>42251</v>
       </c>
@@ -7514,7 +7515,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="196" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="3">
         <v>42251</v>
       </c>
@@ -7552,7 +7553,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="197" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="3">
         <v>42251</v>
       </c>
@@ -7587,7 +7588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
         <v>42251</v>
       </c>
@@ -7626,7 +7627,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="199" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199" s="3">
         <v>42251</v>
       </c>
@@ -7662,7 +7663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200" s="3">
         <v>42258</v>
       </c>
@@ -7692,7 +7693,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="201" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="3">
         <v>42258</v>
       </c>
@@ -7722,7 +7723,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="202" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="3">
         <v>42258</v>
       </c>
@@ -7782,7 +7783,7 @@
         <v>45.5</v>
       </c>
     </row>
-    <row r="204" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="3">
         <v>42258</v>
       </c>
@@ -7808,7 +7809,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="3">
         <v>42258</v>
       </c>
@@ -7832,7 +7833,7 @@
         <v>31.5</v>
       </c>
     </row>
-    <row r="206" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="3">
         <v>42258</v>
       </c>
@@ -7859,7 +7860,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="207" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="3">
         <v>42258</v>
       </c>
@@ -7885,7 +7886,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="208" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="3">
         <v>42258</v>
       </c>
@@ -7911,7 +7912,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="209" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="3">
         <v>42265</v>
       </c>
@@ -7941,7 +7942,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="210" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="3">
         <v>42265</v>
       </c>
@@ -7971,7 +7972,7 @@
         <v>11.5</v>
       </c>
     </row>
-    <row r="211" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="3">
         <v>42265</v>
       </c>
@@ -8034,7 +8035,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="213" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="3">
         <v>42265</v>
       </c>
@@ -8061,7 +8062,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="214" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="3">
         <v>42265</v>
       </c>
@@ -8088,7 +8089,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="3">
         <v>42265</v>
       </c>
@@ -8118,7 +8119,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="216" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="3">
         <v>42265</v>
       </c>
@@ -8145,7 +8146,7 @@
         <v>45.5</v>
       </c>
     </row>
-    <row r="217" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="3">
         <v>42265</v>
       </c>
@@ -8178,7 +8179,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="218" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218" s="3">
         <v>42273</v>
       </c>
@@ -8204,7 +8205,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="219" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="3">
         <v>42273</v>
       </c>
@@ -8230,7 +8231,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="220" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="3">
         <v>42273</v>
       </c>
@@ -8282,7 +8283,7 @@
         <v>16.5</v>
       </c>
     </row>
-    <row r="222" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222" s="3">
         <v>42273</v>
       </c>
@@ -8311,7 +8312,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="223" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="3">
         <v>42273</v>
       </c>
@@ -8340,7 +8341,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="224" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="3">
         <v>42273</v>
       </c>
@@ -8366,7 +8367,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="225" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="3">
         <v>42273</v>
       </c>
@@ -8392,7 +8393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="226" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226" s="3">
         <v>42273</v>
       </c>
@@ -8418,7 +8419,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="227" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227" s="3">
         <v>42279</v>
       </c>
@@ -8444,7 +8445,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228" s="3">
         <v>42279</v>
       </c>
@@ -8470,7 +8471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229" s="3">
         <v>42279</v>
       </c>
@@ -8522,7 +8523,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231" s="3">
         <v>42279</v>
       </c>
@@ -8551,7 +8552,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="232" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232" s="3">
         <v>42279</v>
       </c>
@@ -8578,7 +8579,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="233" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233" s="3">
         <v>42279</v>
       </c>
@@ -8604,7 +8605,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="234" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234" s="3">
         <v>42279</v>
       </c>
@@ -8628,7 +8629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235" s="3">
         <v>42286</v>
       </c>
@@ -8654,7 +8655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236" s="3">
         <v>42286</v>
       </c>
@@ -8680,7 +8681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237" s="3">
         <v>42286</v>
       </c>
@@ -8730,7 +8731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239" s="3">
         <v>42286</v>
       </c>
@@ -8754,7 +8755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240" s="3">
         <v>42286</v>
       </c>
@@ -8778,7 +8779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A241" s="3">
         <v>42286</v>
       </c>
@@ -8803,7 +8804,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q241"/>
+  <autoFilter ref="A1:Q241">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="sucker creek"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:L122">
     <sortCondition ref="A1"/>
   </sortState>

</xml_diff>